<commit_message>
#issue  duplicate value in excel file
</commit_message>
<xml_diff>
--- a/DragonTigerResult.xlsx
+++ b/DragonTigerResult.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,59 +457,119 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>94077</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6 of Heart</t>
+          <t>3 of Dimonds</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>K of Spades</t>
+          <t>A of Spades</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Tiger Won</t>
+          <t>Dragon Won</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>94077</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6 of Heart</t>
+          <t>3 of Dimonds</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>K of Spades</t>
+          <t>A of Spades</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tiger Won</t>
+          <t>Dragon Won</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>94078</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10 of Clubs</t>
+          <t>6 of Spades</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>J of Heart</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Tiger Won</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3 of Dimonds</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A of Spades</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Dragon Won</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>6 of Spades</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>J of Heart</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tiger Won</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9 of Heart</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4 of Spades</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Dragon Won</t>
         </is>

</xml_diff>